<commit_message>
Update Praktek dan Excel
</commit_message>
<xml_diff>
--- a/penjelasan_detail.xlsx
+++ b/penjelasan_detail.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositories\Data_Preparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292944D5-20FC-45CD-93BB-6686704C8CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504490A3-0E22-4C4E-AB9A-9A4861A47962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4D54FE41-69FA-4DD0-9C27-3FB976BDADAB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{4D54FE41-69FA-4DD0-9C27-3FB976BDADAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Membentuk DataFrame" sheetId="1" r:id="rId1"/>
     <sheet name="Deep vs Shallow" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="47">
   <si>
     <t>Pandas</t>
   </si>
@@ -157,13 +158,37 @@
   </si>
   <si>
     <t>shallow copy</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
+  <si>
+    <t>q1</t>
+  </si>
+  <si>
+    <t>q2</t>
+  </si>
+  <si>
+    <t>q3</t>
+  </si>
+  <si>
+    <t>modus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +201,13 @@
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -195,17 +227,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1064,7 +1099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CFC4D64-BC5D-440E-9DB6-23933EC4E17C}">
   <dimension ref="A3:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -1182,4 +1217,221 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3DEDF9F-DBC7-4BBE-9C20-81D542DB0F44}">
+  <dimension ref="B9:N26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D9" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2000</v>
+      </c>
+      <c r="F9" s="3">
+        <v>5000</v>
+      </c>
+      <c r="G9" s="3">
+        <v>6500</v>
+      </c>
+      <c r="H9" s="3">
+        <v>6500</v>
+      </c>
+      <c r="I9" s="3">
+        <v>6500</v>
+      </c>
+      <c r="J9" s="3">
+        <v>7000</v>
+      </c>
+      <c r="K9" s="3">
+        <v>8500</v>
+      </c>
+      <c r="L9" s="3">
+        <v>9000</v>
+      </c>
+      <c r="M9" s="3">
+        <v>10500</v>
+      </c>
+      <c r="N9" s="3">
+        <v>150000000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="3">
+        <f>AVERAGE(D9:N9)</f>
+        <v>13642045.454545455</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="3">
+        <f>MEDIAN(D9:N9)</f>
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="3">
+        <f>_xlfn.STDEV.S((D9:N9))</f>
+        <v>45224817.327687763</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="3">
+        <f>_xlfn.QUARTILE.INC(D9:N9,1)</f>
+        <v>5750</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="3">
+        <f>_xlfn.QUARTILE.INC(D9:N9,2)</f>
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="3">
+        <f>_xlfn.QUARTILE.INC(D9:N9,3)</f>
+        <v>8750</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="3">
+        <f>_xlfn.MODE.SNGL(D9:N9)</f>
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D19" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E19" s="3">
+        <v>2000</v>
+      </c>
+      <c r="F19" s="3">
+        <v>5000</v>
+      </c>
+      <c r="G19" s="3">
+        <v>6500</v>
+      </c>
+      <c r="H19" s="3">
+        <v>6500</v>
+      </c>
+      <c r="I19" s="3">
+        <v>6500</v>
+      </c>
+      <c r="J19" s="3">
+        <v>7000</v>
+      </c>
+      <c r="K19" s="3">
+        <v>8500</v>
+      </c>
+      <c r="L19" s="3">
+        <v>9000</v>
+      </c>
+      <c r="M19" s="3">
+        <v>10500</v>
+      </c>
+      <c r="N19" s="3">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="3">
+        <f>AVERAGE(D19:N19)</f>
+        <v>7045.454545454545</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="3">
+        <f>MEDIAN(D19:N19)</f>
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="3">
+        <f>_xlfn.STDEV.S((D19:N19))</f>
+        <v>3850.0295158254662</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="3">
+        <f>_xlfn.QUARTILE.INC(D19:N19,1)</f>
+        <v>5750</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="3">
+        <f>_xlfn.QUARTILE.INC(D19:N19,2)</f>
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="3">
+        <f>_xlfn.QUARTILE.INC(D19:N19,3)</f>
+        <v>8750</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="3">
+        <f>_xlfn.MODE.SNGL(D19:N19)</f>
+        <v>6500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>